<commit_message>
modify the data structure
</commit_message>
<xml_diff>
--- a/data/curriculum_matrix/人工智能_课程矩阵.xlsx
+++ b/data/curriculum_matrix/人工智能_课程矩阵.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,19 +483,19 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AI201 人工智能导论（必修）</t>
+          <t>EN102 大学英语2（必修）</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>CM201 C语言程序设计（必修）</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>AI202 概率图模型基础（选修）</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>AI202 概率图模型基础（选修）</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>AI301 机器学习（必修）</t>
@@ -503,7 +503,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>AI301 机器学习（必修）</t>
+          <t>AI302 深度学习（必修）</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>AI401 模式识别（必修）</t>
+          <t>AI402 强化学习（选修）</t>
         </is>
       </c>
     </row>
@@ -525,343 +525,235 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EN101 大学英语1（必修）</t>
+          <t>MA102 高等数学A(下)（必修）</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CM201 C语言程序设计（必修）</t>
+          <t>CM203 Python程序设计基础（必修）</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>CM201 C语言程序设计（必修）</t>
+          <t>CM202 C++程序设计基础（必修）</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>AI302 深度学习（必修）</t>
+          <t>AI303 计算机视觉（选修）</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>AI302 深度学习（必修）</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>AI402 强化学习（选修）</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>AI402 强化学习（选修）</t>
-        </is>
-      </c>
+          <t>GE112 音乐鉴赏（选修）</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>EN102 大学英语2（必修）</t>
+          <t>MA101 高等数学A(上)（必修）</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EN102 大学英语2（必修）</t>
+          <t>PE102 大学体育2（必修）</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CM202 C++程序设计基础（必修）</t>
+          <t>CM204 数据结构与算法设计（必修）</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>CM202 C++程序设计基础（必修）</t>
+          <t>GE102 经济学原理（选修）</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>AI303 计算机视觉（选修）</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>AI303 计算机视觉（选修）</t>
-        </is>
-      </c>
+          <t>AI304 自然语言处理（选修）</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MA101 高等数学A(上)（必修）</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>MA101 高等数学A(上)（必修）</t>
-        </is>
-      </c>
+          <t>ML101 军事理论（必修）</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CM203 Python程序设计基础（必修）</t>
+          <t>CM205 离散数学（必修）</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>CM203 Python程序设计基础（必修）</t>
+          <t>MA202 概率论与数理统计（必修）</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>AI304 自然语言处理（选修）</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>AI304 自然语言处理（选修）</t>
-        </is>
-      </c>
+          <t>CM206 计算机组成原理（必修）</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MA102 高等数学A(下)（必修）</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>MA102 高等数学A(下)（必修）</t>
-        </is>
-      </c>
+          <t>PE101 大学体育1（必修）</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CM204 数据结构与算法设计（必修）</t>
+          <t>EN103 大学英语3（必修）</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>CM204 数据结构与算法设计（必修）</t>
+          <t>PH102 大学物理A(下)（必修）</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>CM206 计算机组成原理（必修）</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>CM206 计算机组成原理（必修）</t>
-        </is>
-      </c>
+          <t>CM207 操作系统原理（必修）</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ML101 军事理论（必修）</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ML101 军事理论（必修）</t>
-        </is>
-      </c>
+          <t>PH101 大学物理A(上)（必修）</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CM205 离散数学（必修）</t>
+          <t>EN104 大学英语4（必修）</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>CM205 离散数学（必修）</t>
+          <t>ZX102 马克思主义基本原理（必修）</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>CM207 操作系统原理（必修）</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>CM207 操作系统原理（必修）</t>
-        </is>
-      </c>
+          <t>CM208 数据库系统基础（必修）</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>PE101 大学体育1（必修）</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>PE101 大学体育1（必修）</t>
-        </is>
-      </c>
+          <t>XL101 大学生心理健康教育（必修）</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>EN103 大学英语3（必修）</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>EN103 大学英语3（必修）</t>
-        </is>
-      </c>
+          <t>GE101 艺术欣赏（选修）</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
-          <t>CM208 数据库系统基础（必修）</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>CM208 数据库系统基础（必修）</t>
-        </is>
-      </c>
+          <t>CM209 计算机网络基础（必修）</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>PE102 大学体育2（必修）</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>PE102 大学体育2（必修）</t>
-        </is>
-      </c>
+          <t>ZX101 思想道德与法治（必修）</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>EN104 大学英语4（必修）</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>EN104 大学英语4（必修）</t>
-        </is>
-      </c>
+          <t>GE103 摄影基础（选修）</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CM209 计算机网络基础（必修）</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>CM209 计算机网络基础（必修）</t>
-        </is>
-      </c>
+          <t>CM210 软件工程导论（必修）</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>PH101 大学物理A(上)（必修）</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>PH101 大学物理A(上)（必修）</t>
-        </is>
-      </c>
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>GE101 艺术欣赏（选修）</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>GE101 艺术欣赏（选修）</t>
-        </is>
-      </c>
+          <t>GE104 影视鉴赏（选修）</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
-          <t>CM210 软件工程导论（必修）</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>CM210 软件工程导论（必修）</t>
-        </is>
-      </c>
+          <t>CS301 数据库系统原理（必修）</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>XL101 大学生心理健康教育（必修）</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>XL101 大学生心理健康教育（必修）</t>
-        </is>
-      </c>
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>GE102 经济学原理（选修）</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>GE102 经济学原理（选修）</t>
-        </is>
-      </c>
+          <t>GE105 管理学基础（选修）</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr">
         <is>
-          <t>CS301 数据库系统原理（必修）</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>CS301 数据库系统原理（必修）</t>
-        </is>
-      </c>
+          <t>GE108 哲学与人生（选修）</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>ZX101 思想道德与法治（必修）</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>ZX101 思想道德与法治（必修）</t>
-        </is>
-      </c>
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>GE103 摄影基础（选修）</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>GE103 摄影基础（选修）</t>
-        </is>
-      </c>
+          <t>GE106 心理学导论（选修）</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
-          <t>GE108 哲学与人生（选修）</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>GE108 哲学与人生（选修）</t>
-        </is>
-      </c>
+          <t>GE109 逻辑思维训练（选修）</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
     </row>
@@ -870,24 +762,16 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>GE104 影视鉴赏（选修）</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>GE104 影视鉴赏（选修）</t>
-        </is>
-      </c>
+          <t>GE107 统计学基础（选修）</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr"/>
       <c r="E13" t="inlineStr">
         <is>
-          <t>GE109 逻辑思维训练（选修）</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>GE109 逻辑思维训练（选修）</t>
-        </is>
-      </c>
+          <t>GE110 创新创业基础（选修）</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
     </row>
@@ -896,24 +780,16 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>GE105 管理学基础（选修）</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>GE105 管理学基础（选修）</t>
-        </is>
-      </c>
+          <t>HX101 中国近现代史纲要（必修）</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
-          <t>GE110 创新创业基础（选修）</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>GE110 创新创业基础（选修）</t>
-        </is>
-      </c>
+          <t>GE111 书法艺术（选修）</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr"/>
     </row>
@@ -922,24 +798,16 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>GE106 心理学导论（选修）</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>GE106 心理学导论（选修）</t>
-        </is>
-      </c>
+          <t>MA201 线性代数（必修）</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr"/>
       <c r="E15" t="inlineStr">
         <is>
-          <t>GE111 书法艺术（选修）</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>GE111 书法艺术（选修）</t>
-        </is>
-      </c>
+          <t>GE113 世界文明史（选修）</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr"/>
       <c r="H15" t="inlineStr"/>
     </row>
@@ -948,24 +816,16 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>GE107 统计学基础（选修）</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>GE107 统计学基础（选修）</t>
-        </is>
-      </c>
+          <t>PE103 大学体育3（必修）</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr">
         <is>
-          <t>GE112 音乐鉴赏（选修）</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>GE112 音乐鉴赏（选修）</t>
-        </is>
-      </c>
+          <t>GE114 环境与可持续发展（选修）</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr"/>
       <c r="H16" t="inlineStr"/>
     </row>
@@ -974,200 +834,88 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>HX101 中国近现代史纲要（必修）</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>HX101 中国近现代史纲要（必修）</t>
-        </is>
-      </c>
+          <t>PE104 大学体育4（必修）</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr">
         <is>
-          <t>GE113 世界文明史（选修）</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>GE113 世界文明史（选修）</t>
-        </is>
-      </c>
+          <t>GE115 法律基础与法治思维（选修）</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>MA201 线性代数（必修）</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>MA201 线性代数（必修）</t>
-        </is>
-      </c>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
       <c r="E18" t="inlineStr">
         <is>
-          <t>GE114 环境与可持续发展（选修）</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>GE114 环境与可持续发展（选修）</t>
-        </is>
-      </c>
+          <t>GE116 公共演讲与表达（选修）</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr"/>
       <c r="H18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>MA202 概率论与数理统计（必修）</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>MA202 概率论与数理统计（必修）</t>
-        </is>
-      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>GE115 法律基础与法治思维（选修）</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>GE115 法律基础与法治思维（选修）</t>
-        </is>
-      </c>
+          <t>GE117 职业生涯规划（选修）</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr"/>
       <c r="H19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>PE103 大学体育3（必修）</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>PE103 大学体育3（必修）</t>
-        </is>
-      </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>GE116 公共演讲与表达（选修）</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>GE116 公共演讲与表达（选修）</t>
-        </is>
-      </c>
+          <t>GE118 项目管理基础（选修）</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>PE104 大学体育4（必修）</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>PE104 大学体育4（必修）</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>GE117 职业生涯规划（选修）</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>GE117 职业生涯规划（选修）</t>
-        </is>
-      </c>
+          <t>GE119 城市与社会发展（选修）</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr"/>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>PH102 大学物理A(下)（必修）</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>PH102 大学物理A(下)（必修）</t>
-        </is>
-      </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>GE118 项目管理基础（选修）</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>GE118 项目管理基础（选修）</t>
-        </is>
-      </c>
+          <t>GE120 人工智能与社会（选修）</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr"/>
-      <c r="B23" t="inlineStr"/>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>ZX102 马克思主义基本原理（必修）</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>ZX102 马克思主义基本原理（必修）</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>GE119 城市与社会发展（选修）</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>GE119 城市与社会发展（选修）</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr"/>
-      <c r="C24" t="inlineStr"/>
-      <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>GE120 人工智能与社会（选修）</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>GE120 人工智能与社会（选修）</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>